<commit_message>
0-comparisons, ring name, subvector synonyms
</commit_message>
<xml_diff>
--- a/wip.xlsx
+++ b/wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam.DYALOG\Documents\APLcart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9410AB3B-827B-4C26-B76F-F33F5F0EEA55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286EAADB-89A3-4B33-8256-B0A68DE6310B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="3510" windowWidth="26670" windowHeight="12285" xr2:uid="{C77C04FD-10F8-4476-8FD3-CDE47491BC93}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="1551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="1552">
   <si>
     <t>SYNTAX</t>
   </si>
@@ -4734,6 +4734,9 @@
   </si>
   <si>
     <t>(1,⍨¯1↓2≠⌿⊢↑⍨1+≢)Yv</t>
+  </si>
+  <si>
+    <t>segmented partitioned sub-vectors</t>
   </si>
 </sst>
 </file>
@@ -5141,8 +5144,8 @@
   <dimension ref="A1:J478"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B367" sqref="B367"/>
+      <pane ySplit="1" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B372" sqref="B372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -14554,9 +14557,17 @@
       <c r="B371" s="3" t="s">
         <v>1546</v>
       </c>
-      <c r="E371" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>FinnAPL</v>
+      <c r="C371" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D371" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="F371" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="G371" s="3" t="s">
+        <v>1551</v>
       </c>
       <c r="H371" s="3">
         <v>0</v>

</xml_diff>